<commit_message>
Não abre o chamado
</commit_message>
<xml_diff>
--- a/Cleintes digisac novo.xlsx
+++ b/Cleintes digisac novo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Elton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Victor Cals</t>
   </si>
 </sst>
 </file>
@@ -238,16 +235,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,15 +260,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>5541998306017</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>41992452510</v>
+        <v>41998306017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>